<commit_message>
Removed (Inactive) String from pdf names & Removed char S from Medical Recods
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -87,7 +87,7 @@
     <t>https://masmdvapp.eclinicalweb.com/mobiledoc/jsp/webemr/login/newLogin.jsp</t>
   </si>
   <si>
-    <t>ab,ac</t>
+    <t>ab,ca</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -236,7 +236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
login selector issue fixed
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Damco RPA Projects\Morgan_Records_Process_Wave_2\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -30,21 +30,27 @@
     <t>Description</t>
   </si>
   <si>
+    <t>WC_Name</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>Windows Credential Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://masmdvapp.eclinicalweb.com/mobiledoc/jsp/webemr/login/newLogin.jsp</t>
+  </si>
+  <si>
     <t>MaxRetry</t>
   </si>
   <si>
     <t>Maximum retry attempts for certain workflows</t>
   </si>
   <si>
-    <t>WC_Name</t>
-  </si>
-  <si>
-    <t>Windows Credential Name</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Timeout</t>
   </si>
   <si>
@@ -54,7 +60,7 @@
     <t>Alphabets</t>
   </si>
   <si>
-    <t>MR</t>
+    <t>ge, gh, gi, gn, go, gr, gu, gw, ha</t>
   </si>
   <si>
     <t>Alphabets which needs to be searched for should be saparated by Comma</t>
@@ -63,15 +69,18 @@
     <t>Fresh_Run</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Type No if the bot has already downloaded the Patient Details and needed to run afterwards</t>
+  </si>
+  <si>
     <t>File_Path</t>
   </si>
   <si>
     <t>Path of the file where in the details are already present</t>
   </si>
   <si>
-    <t>Type No if the bot has already downloaded the Patient Details and needed to run afterwards</t>
-  </si>
-  <si>
     <t>Sheet_Name</t>
   </si>
   <si>
@@ -81,25 +90,19 @@
     <t>Name of the sheet/tab where in the patient details are present</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>https://masmdvapp.eclinicalweb.com/mobiledoc/jsp/webemr/login/newLogin.jsp</t>
-  </si>
-  <si>
-    <t>ab,ca</t>
+    <t>C:\Users\User\Desktop\Damco RPA Projects\Morgan_Records_Process_Wave_2\Output\Morgan Records Report 17 Nov 2020.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -107,7 +110,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -133,11 +136,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -201,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -236,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -411,11 +414,6 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -424,114 +422,117 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="85.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60000</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>60000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>